<commit_message>
Empezamos con la produccion
</commit_message>
<xml_diff>
--- a/public/informes/1116/1116_1_5 TAPA 200 ML MONOPARED PLANA/1116_ 1_ 5 2021-10-07.xlsx
+++ b/public/informes/1116/1116_1_5 TAPA 200 ML MONOPARED PLANA/1116_ 1_ 5 2021-10-07.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.26.0.12\samba-share\CARPETA COMÚ\INFORMES MOTLLES\Terminados\1116\1116_1_5 TAPA 200 ML MONOPARED PLANA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.26.0.13\CompartidaFabrica\INFORMES MOTLLES\Terminados\1116\1116_1_5 TAPA 200 ML MONOPARED PLANA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>DENOMINACIÓ</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>NO HI HA UNYETA A LA COLADA I NO CAU. EL MOTLLE PERD AIGUA PER LA ZONA DE LA CREMALLERA. CAL REAJUSTAR MOTLLE, REBAVA PARTAGE I CONO, ENS ESTAN RECLAMANT MOSTRES DES DEL DEPARTAMENT COMERCIAL.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15/02/2021</t>
   </si>
   <si>
     <t>Se ha fabricado e instalado el expulsor arrape del centro. 
@@ -80,28 +77,16 @@
 Reparamos fuga de agua detectada en el punzon fijo central de la tapa.</t>
   </si>
   <si>
-    <t>17/02/2021 Inyeccion</t>
-  </si>
-  <si>
     <t>Rebaba y suciedad en la zona del ribete.</t>
   </si>
   <si>
     <t>NO OK</t>
   </si>
   <si>
-    <t>29/04/2021 Taller</t>
-  </si>
-  <si>
-    <t>03/5/2021 Taller</t>
-  </si>
-  <si>
     <t>Segons injeccio: Esta clavat . (Solo parte movil)</t>
   </si>
   <si>
     <t>Desmontar completo, todas las placas, la rosca esta fija y no se mueve.- Intentar aflojar rosca de varias maneras.- se ha movido un poco, pero va muy dura y hay peligro de estropear parte de la pieza o engranaje. Hablado con M. Serrano y mandar parte a Cornella.</t>
-  </si>
-  <si>
-    <t>13/05/2021 del  Taller a Cornella (resto de placas)</t>
   </si>
   <si>
     <t>Para fabricar y montar la nueva camisa.</t>
@@ -113,16 +98,7 @@
 Camisa casquillo de expulsion en 1.2344 templada y revenida a 50/52.</t>
   </si>
   <si>
-    <t>17/06/2021 Injeccio</t>
-  </si>
-  <si>
-    <t>21/06/2021 Taller</t>
-  </si>
-  <si>
     <t>Injeccio:Surten les peçes brutes per dintre el costat boca. S'ha desmontat la placa expulsora peçes, tot net. Encara surten brutes. La grasa surt de dintre el noyo. Es baixa part movil per netejar (ordre Dani) Es baixan mostres.</t>
-  </si>
-  <si>
-    <t>22/06/2021 de Taller a Cornella</t>
   </si>
   <si>
     <t>Taller:reparar noyo central roto, desclavar desenroscado, comprobar circuito refrigeracion ambos lados.</t>
@@ -148,24 +124,12 @@
     <t>Este molde solo tiene una pieza activa, la otra esta anulada. Desmontar parte de expulsión completa.- limpiar molde.- quitar golpes en placas, extraer casquillo anulado y limpiar lleno de corrosión, extraer casquillo camisa rosca porta juntas del circuito esta corroído, habría que reconstruir.- poner juntas torticas todas nuevas.- comprobar refrigeración ok. Engrasar y posicionar cremallera y engranaje. Cerrar molde. Hay juego desplazado en el noyo interior.</t>
   </si>
   <si>
-    <t>03/05/2021 del  Taller a Cornella (solo piña versión y placa)</t>
-  </si>
-  <si>
-    <t>21/07/2021 Taller</t>
-  </si>
-  <si>
     <t>Injeccion:Sha de repasar la rosca de la pinya on es colla el pistó.</t>
   </si>
   <si>
     <t>Desmontar la piña y estraer esparrago, repasar rosca y volver a montar.</t>
   </si>
   <si>
-    <t>21/07/2021 de Taller a Pasillo.- Estanteria amb ubicación ocupada.</t>
-  </si>
-  <si>
-    <t>01/09/2021 Taller procedente de Injeccio</t>
-  </si>
-  <si>
     <t>Injeccion:S'ha clavat la cremallera encara en produccio.</t>
   </si>
   <si>
@@ -175,16 +139,7 @@
     <t>Desmontar completo, todas las placas, la parte central delantera esta limpia, la rosca hay un trozo que va dura, desmontar y esta mas o menos limpia, en la zona del piñon de atras, hay depositado bastante grasa ya liquada, que por deduccion al no tener salida con el movimiento pasa a la parte posterior manchando la pieza. Habria que realizar un conducto de drenaje en la parte trasera inferior del alojamiento del piñon, asi como una salida de aire lateral al noyo central. y en la superficie del ajuste un relieve para que sirva de deposito de engrase. Al montar molde se clava el desenroscado y se rompe el noyo central, consultar con Serrano y mandar a Cornella.</t>
   </si>
   <si>
-    <t>01/09/2021 de taller a Cornella. (solo rosca patron y camisa)</t>
-  </si>
-  <si>
     <t>Recepcionada parte procedente de Cornella.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/09/2021 Taller </t>
-  </si>
-  <si>
-    <t>03/09/2021 de taller a Injeccion</t>
   </si>
   <si>
     <t>Camisa gripada en noyo central</t>
@@ -867,8 +822,8 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,30 +912,30 @@
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
+      <c r="B7" s="5">
+        <v>44242</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F7" s="5">
         <v>44244</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>16</v>
+      <c r="A8" s="5">
+        <v>44244</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="12"/>
@@ -994,63 +949,63 @@
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>19</v>
+      <c r="A10" s="5">
+        <v>44315</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="17" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>44319</v>
+      </c>
+      <c r="B11" s="5">
+        <v>44319</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>22</v>
-      </c>
       <c r="E11" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>23</v>
+      <c r="A12" s="5">
+        <v>44329</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="12"/>
@@ -1064,44 +1019,44 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>27</v>
+      <c r="A14" s="15">
+        <v>44364</v>
+      </c>
+      <c r="B14" s="15">
+        <v>44368</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>29</v>
+      <c r="A15" s="5">
+        <v>44369</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="17" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="12"/>
@@ -1115,43 +1070,43 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>38</v>
+      <c r="A17" s="15">
+        <v>44398</v>
+      </c>
+      <c r="B17" s="15">
+        <v>44398</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>42</v>
+      <c r="A18" s="15">
+        <v>44440</v>
+      </c>
+      <c r="B18" s="15">
+        <v>44440</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="26"/>
@@ -1163,27 +1118,27 @@
         <v>44441</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>48</v>
+      <c r="A20" s="15">
+        <v>44442</v>
+      </c>
+      <c r="B20" s="15">
+        <v>44441</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="28"/>
@@ -1196,7 +1151,7 @@
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="17" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="32"/>

</xml_diff>